<commit_message>
add all Football Games
</commit_message>
<xml_diff>
--- a/data/London Games/London_Games_2020.xlsx
+++ b/data/London Games/London_Games_2020.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timlehmann/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timlehmann/StudyProject2024-1/data/London Games/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E75652-5901-C246-9774-A0ACA387008E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC91465F-DA4F-C24B-A10B-EE7E97176256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{4D55FC88-3B05-B643-8608-574EA16C2234}"/>
+    <workbookView xWindow="-2680" yWindow="-25440" windowWidth="34400" windowHeight="20820" xr2:uid="{4D55FC88-3B05-B643-8608-574EA16C2234}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="82">
   <si>
     <t>Date</t>
   </si>
@@ -148,13 +148,172 @@
   </si>
   <si>
     <t xml:space="preserve">Date </t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>FA Cup</t>
+  </si>
+  <si>
+    <t>Derby County</t>
+  </si>
+  <si>
+    <t>Charlton Athletic</t>
+  </si>
+  <si>
+    <t>Nottingham Forest</t>
+  </si>
+  <si>
+    <t>Middlesbrough</t>
+  </si>
+  <si>
+    <t>Plymouth Argyle</t>
+  </si>
+  <si>
+    <t>EFL Cup</t>
+  </si>
+  <si>
+    <t>FC Barnlsey</t>
+  </si>
+  <si>
+    <t>Sheffield Wed.</t>
+  </si>
+  <si>
+    <t>Hull City</t>
+  </si>
+  <si>
+    <t>Doncaster Rov</t>
+  </si>
+  <si>
+    <t>League One</t>
+  </si>
+  <si>
+    <t>AFC Sunderland</t>
+  </si>
+  <si>
+    <t>Wigan Athletic</t>
+  </si>
+  <si>
+    <t>Oxford United</t>
+  </si>
+  <si>
+    <t>Fleetwood Town</t>
+  </si>
+  <si>
+    <t>MK Dons</t>
+  </si>
+  <si>
+    <t>AFC Wimbledon</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>Championship</t>
+  </si>
+  <si>
+    <t>Barnsley</t>
+  </si>
+  <si>
+    <t>Huddersfield</t>
+  </si>
+  <si>
+    <t>Blackburn</t>
+  </si>
+  <si>
+    <t>Luton Town</t>
+  </si>
+  <si>
+    <t>Swansea</t>
+  </si>
+  <si>
+    <t>Preston NE</t>
+  </si>
+  <si>
+    <t>Brentfort</t>
+  </si>
+  <si>
+    <t>QPR</t>
+  </si>
+  <si>
+    <t>FC Millwall</t>
+  </si>
+  <si>
+    <t>Birmingham City</t>
+  </si>
+  <si>
+    <t>Cardiff City</t>
+  </si>
+  <si>
+    <t>FC Reading</t>
+  </si>
+  <si>
+    <t>Olympiakos Piräus</t>
+  </si>
+  <si>
+    <t>Europa League</t>
+  </si>
+  <si>
+    <t>FC Dundalk</t>
+  </si>
+  <si>
+    <t>Molde FK</t>
+  </si>
+  <si>
+    <t>Rapid Wien</t>
+  </si>
+  <si>
+    <t>RB Leipzig</t>
+  </si>
+  <si>
+    <t>Champions League</t>
+  </si>
+  <si>
+    <t>Bayern München</t>
+  </si>
+  <si>
+    <t>FC Sevilla</t>
+  </si>
+  <si>
+    <t>Stade Rennes</t>
+  </si>
+  <si>
+    <t>FK Krasnodar</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Wales</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Irland</t>
+  </si>
+  <si>
+    <t>Belgien</t>
+  </si>
+  <si>
+    <t>Nations League</t>
+  </si>
+  <si>
+    <t>Dänemark</t>
+  </si>
+  <si>
+    <t>Island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tottenham </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -170,13 +329,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -191,14 +363,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -533,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBA24EEF-0B53-A64E-9F41-ED31D933E633}">
-  <dimension ref="B2:I94"/>
+  <dimension ref="B2:P157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,28 +717,33 @@
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="H4" t="s">
         <v>28</v>
       </c>
@@ -573,52 +751,76 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="2">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
         <v>43831</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" t="s">
         <v>4</v>
       </c>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
       <c r="H5" s="1" cm="1">
-        <f t="array" ref="H5:H68">_xlfn.UNIQUE(B5:B94)</f>
+        <f t="array" ref="H5:H109">_xlfn.UNIQUE(B5:B157)</f>
         <v>43831</v>
       </c>
       <c r="I5">
-        <f>COUNTIF(B$5:B$94,H5)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="2">
+        <f>COUNTIF(B$5:B$157,H5)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
         <v>43831</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="1">
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="4">
         <v>43841</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I68" si="0">COUNTIF(B$5:B$94,H6)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="2">
+        <f t="shared" ref="I6:I69" si="0">COUNTIF(B$5:B$157,H6)</f>
+        <v>4</v>
+      </c>
+      <c r="L6" s="1">
         <v>43841</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="M6" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="N6" t="s">
+        <v>7</v>
+      </c>
+      <c r="O6" t="s">
+        <v>81</v>
+      </c>
+      <c r="P6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>43841</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
         <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>26</v>
       </c>
       <c r="H7" s="1">
         <v>43848</v>
@@ -627,16 +829,34 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="2">
+      <c r="L7" s="1">
+        <v>43862</v>
+      </c>
+      <c r="M7" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" t="s">
+        <v>32</v>
+      </c>
+      <c r="P7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
         <v>43841</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" t="s">
         <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
       </c>
       <c r="H8" s="1">
         <v>43851</v>
@@ -645,34 +865,70 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="2">
+      <c r="L8" s="1">
+        <v>44038</v>
+      </c>
+      <c r="M8" t="s">
+        <v>5</v>
+      </c>
+      <c r="N8" t="s">
+        <v>7</v>
+      </c>
+      <c r="O8" t="s">
+        <v>6</v>
+      </c>
+      <c r="P8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
         <v>43841</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" t="s">
         <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
       </c>
       <c r="H9" s="1">
         <v>43852</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="L9" s="1">
+        <v>44142</v>
+      </c>
+      <c r="M9" t="s">
+        <v>6</v>
+      </c>
+      <c r="N9" t="s">
+        <v>7</v>
+      </c>
+      <c r="O9" t="s">
+        <v>3</v>
+      </c>
+      <c r="P9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
         <v>43848</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" t="s">
         <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
       </c>
       <c r="H10" s="1">
         <v>43859</v>
@@ -682,33 +938,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="2">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
         <v>43848</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="1">
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="4">
         <v>43862</v>
       </c>
       <c r="I11">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B12" s="1">
         <v>43851</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" t="s">
         <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>26</v>
       </c>
       <c r="H12" s="1">
         <v>43863</v>
@@ -718,15 +980,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="2">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B13" s="1">
         <v>43851</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" t="s">
         <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>26</v>
       </c>
       <c r="H13" s="1">
         <v>43877</v>
@@ -736,15 +1001,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="2">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B14" s="1">
         <v>43852</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" t="s">
         <v>14</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
       </c>
       <c r="H14" s="1">
         <v>43878</v>
@@ -754,33 +1022,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="2">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B15" s="1">
         <v>43859</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" t="s">
         <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
       </c>
       <c r="H15" s="1">
         <v>43883</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
         <v>43862</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" t="s">
         <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
       </c>
       <c r="H16" s="1">
         <v>43884</v>
@@ -791,32 +1065,38 @@
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>43862</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" t="s">
         <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>26</v>
       </c>
       <c r="H17" s="1">
         <v>43890</v>
       </c>
       <c r="I17">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>43863</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" t="s">
         <v>16</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
       </c>
       <c r="H18" s="1">
         <v>43891</v>
@@ -827,32 +1107,38 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>43877</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="1">
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="5">
         <v>43897</v>
       </c>
       <c r="I19">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>43878</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" t="s">
         <v>17</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
       </c>
       <c r="H20" s="1">
         <v>43898</v>
@@ -863,14 +1149,17 @@
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>43883</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" t="s">
         <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
       </c>
       <c r="H21" s="1">
         <v>44001</v>
@@ -881,32 +1170,38 @@
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>43883</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" t="s">
         <v>18</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
       </c>
       <c r="H22" s="1">
         <v>44002</v>
       </c>
       <c r="I22">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>43884</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" t="s">
         <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
       </c>
       <c r="H23" s="1">
         <v>44005</v>
@@ -917,14 +1212,17 @@
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>43890</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" t="s">
         <v>3</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" t="s">
         <v>13</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
       </c>
       <c r="H24" s="1">
         <v>44007</v>
@@ -935,14 +1233,17 @@
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>43891</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" t="s">
         <v>19</v>
+      </c>
+      <c r="E25" t="s">
+        <v>26</v>
       </c>
       <c r="H25" s="1">
         <v>44011</v>
@@ -953,14 +1254,17 @@
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>43897</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D26" t="s">
         <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>26</v>
       </c>
       <c r="H26" s="1">
         <v>44013</v>
@@ -971,32 +1275,38 @@
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>43897</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" t="s">
         <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>26</v>
       </c>
       <c r="H27" s="1">
         <v>44016</v>
       </c>
       <c r="I27">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>43898</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" t="s">
         <v>7</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" t="s">
         <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
       </c>
       <c r="H28" s="1">
         <v>44018</v>
@@ -1007,14 +1317,17 @@
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>44001</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" t="s">
         <v>9</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" t="s">
         <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
       </c>
       <c r="H29" s="1">
         <v>44019</v>
@@ -1025,14 +1338,17 @@
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>44002</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" t="s">
         <v>19</v>
+      </c>
+      <c r="E30" t="s">
+        <v>26</v>
       </c>
       <c r="H30" s="1">
         <v>44020</v>
@@ -1043,14 +1359,17 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>44005</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" t="s">
         <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>26</v>
       </c>
       <c r="H31" s="1">
         <v>44024</v>
@@ -1061,14 +1380,17 @@
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>44007</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" t="s">
         <v>16</v>
+      </c>
+      <c r="E32" t="s">
+        <v>26</v>
       </c>
       <c r="H32" s="1">
         <v>44026</v>
@@ -1079,14 +1401,17 @@
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>44011</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" t="s">
         <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>26</v>
       </c>
       <c r="H33" s="1">
         <v>44027</v>
@@ -1097,14 +1422,17 @@
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>44013</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" t="s">
         <v>14</v>
+      </c>
+      <c r="E34" t="s">
+        <v>26</v>
       </c>
       <c r="H34" s="1">
         <v>44028</v>
@@ -1115,14 +1443,17 @@
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>44013</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" t="s">
         <v>3</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" t="s">
         <v>7</v>
+      </c>
+      <c r="E35" t="s">
+        <v>26</v>
       </c>
       <c r="H35" s="1">
         <v>44029</v>
@@ -1133,14 +1464,17 @@
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>44016</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" t="s">
         <v>20</v>
+      </c>
+      <c r="E36" t="s">
+        <v>26</v>
       </c>
       <c r="H36" s="1">
         <v>44031</v>
@@ -1151,16 +1485,19 @@
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>44018</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" t="s">
         <v>12</v>
       </c>
-      <c r="H37" s="1">
+      <c r="E37" t="s">
+        <v>26</v>
+      </c>
+      <c r="H37" s="4">
         <v>44038</v>
       </c>
       <c r="I37">
@@ -1169,14 +1506,17 @@
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>44019</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" t="s">
         <v>6</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" t="s">
         <v>7</v>
+      </c>
+      <c r="E38" t="s">
+        <v>26</v>
       </c>
       <c r="H38" s="1">
         <v>44086</v>
@@ -1187,14 +1527,17 @@
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>44019</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" t="s">
         <v>5</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" t="s">
         <v>21</v>
+      </c>
+      <c r="E39" t="s">
+        <v>26</v>
       </c>
       <c r="H39" s="1">
         <v>44087</v>
@@ -1205,32 +1548,38 @@
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>44020</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" t="s">
         <v>3</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" t="s">
         <v>8</v>
+      </c>
+      <c r="E40" t="s">
+        <v>26</v>
       </c>
       <c r="H40" s="1">
         <v>44093</v>
       </c>
       <c r="I40">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>44024</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" t="s">
         <v>9</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" t="s">
         <v>5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>26</v>
       </c>
       <c r="H41" s="1">
         <v>44094</v>
@@ -1241,14 +1590,17 @@
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>44026</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" t="s">
         <v>14</v>
+      </c>
+      <c r="E42" t="s">
+        <v>26</v>
       </c>
       <c r="H42" s="1">
         <v>44100</v>
@@ -1259,14 +1611,17 @@
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>44027</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" t="s">
         <v>10</v>
+      </c>
+      <c r="E43" t="s">
+        <v>26</v>
       </c>
       <c r="H43" s="1">
         <v>44101</v>
@@ -1277,14 +1632,17 @@
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>44028</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" t="s">
         <v>17</v>
+      </c>
+      <c r="E44" t="s">
+        <v>26</v>
       </c>
       <c r="H44" s="1">
         <v>44102</v>
@@ -1295,32 +1653,38 @@
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>44029</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" t="s">
         <v>3</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" t="s">
         <v>20</v>
+      </c>
+      <c r="E45" t="s">
+        <v>26</v>
       </c>
       <c r="H45" s="1">
         <v>44107</v>
       </c>
       <c r="I45">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>44031</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" t="s">
         <v>9</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" t="s">
         <v>21</v>
+      </c>
+      <c r="E46" t="s">
+        <v>26</v>
       </c>
       <c r="H46" s="1">
         <v>44108</v>
@@ -1331,32 +1695,38 @@
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>44038</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="D47" t="s">
         <v>20</v>
+      </c>
+      <c r="E47" t="s">
+        <v>26</v>
       </c>
       <c r="H47" s="1">
         <v>44121</v>
       </c>
       <c r="I47">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>44038</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" t="s">
         <v>7</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" t="s">
         <v>19</v>
+      </c>
+      <c r="E48" t="s">
+        <v>26</v>
       </c>
       <c r="H48" s="1">
         <v>44122</v>
@@ -1367,14 +1737,17 @@
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>44038</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" t="s">
         <v>6</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" t="s">
         <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>26</v>
       </c>
       <c r="H49" s="1">
         <v>44128</v>
@@ -1385,14 +1758,17 @@
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>44038</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" t="s">
         <v>22</v>
+      </c>
+      <c r="E50" t="s">
+        <v>26</v>
       </c>
       <c r="H50" s="1">
         <v>44129</v>
@@ -1403,14 +1779,17 @@
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>44086</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" t="s">
         <v>23</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" t="s">
         <v>5</v>
+      </c>
+      <c r="E51" t="s">
+        <v>26</v>
       </c>
       <c r="H51" s="1">
         <v>44136</v>
@@ -1421,14 +1800,17 @@
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>44086</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" t="s">
         <v>3</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" t="s">
         <v>18</v>
+      </c>
+      <c r="E52" t="s">
+        <v>26</v>
       </c>
       <c r="H52" s="1">
         <v>44137</v>
@@ -1439,32 +1821,38 @@
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>44087</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" t="s">
         <v>12</v>
       </c>
-      <c r="H53" s="1">
+      <c r="E53" t="s">
+        <v>26</v>
+      </c>
+      <c r="H53" s="4">
         <v>44142</v>
       </c>
       <c r="I53">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B54" s="1">
+        <v>44093</v>
+      </c>
+      <c r="C54" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B54" s="2">
-        <v>44093</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>3</v>
+      <c r="E54" t="s">
+        <v>26</v>
       </c>
       <c r="H54" s="1">
         <v>44143</v>
@@ -1475,32 +1863,38 @@
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>44094</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" t="s">
         <v>7</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" t="s">
         <v>10</v>
+      </c>
+      <c r="E55" t="s">
+        <v>26</v>
       </c>
       <c r="H55" s="1">
         <v>44156</v>
       </c>
       <c r="I55">
-        <f t="shared" si="0"/>
+        <f>COUNTIF(B$5:B$157,H55)</f>
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>44100</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" t="s">
         <v>6</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" t="s">
         <v>12</v>
+      </c>
+      <c r="E56" t="s">
+        <v>26</v>
       </c>
       <c r="H56" s="1">
         <v>44157</v>
@@ -1511,14 +1905,17 @@
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>44101</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C57" t="s">
         <v>9</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" t="s">
         <v>18</v>
+      </c>
+      <c r="E57" t="s">
+        <v>26</v>
       </c>
       <c r="H57" s="1">
         <v>44162</v>
@@ -1529,14 +1926,17 @@
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>44101</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C58" t="s">
         <v>3</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="D58" t="s">
         <v>19</v>
+      </c>
+      <c r="E58" t="s">
+        <v>26</v>
       </c>
       <c r="H58" s="1">
         <v>44164</v>
@@ -1547,14 +1947,17 @@
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>44102</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" t="s">
         <v>23</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" t="s">
         <v>22</v>
+      </c>
+      <c r="E59" t="s">
+        <v>26</v>
       </c>
       <c r="H59" s="1">
         <v>44165</v>
@@ -1565,14 +1968,17 @@
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>44107</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" t="s">
         <v>7</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="D60" t="s">
         <v>6</v>
+      </c>
+      <c r="E60" t="s">
+        <v>26</v>
       </c>
       <c r="H60" s="1">
         <v>44170</v>
@@ -1583,14 +1989,17 @@
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>44108</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" t="s">
         <v>5</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="D61" t="s">
         <v>11</v>
+      </c>
+      <c r="E61" t="s">
+        <v>26</v>
       </c>
       <c r="H61" s="1">
         <v>44171</v>
@@ -1601,14 +2010,17 @@
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>44121</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" t="s">
         <v>7</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="D62" t="s">
         <v>13</v>
+      </c>
+      <c r="E62" t="s">
+        <v>26</v>
       </c>
       <c r="H62" s="1">
         <v>44178</v>
@@ -1619,14 +2031,17 @@
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B63" s="2">
+      <c r="B63" s="1">
         <v>44122</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" t="s">
         <v>6</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" t="s">
         <v>15</v>
+      </c>
+      <c r="E63" t="s">
+        <v>26</v>
       </c>
       <c r="H63" s="1">
         <v>44181</v>
@@ -1637,14 +2052,17 @@
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B64" s="2">
+      <c r="B64" s="1">
         <v>44122</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C64" t="s">
         <v>9</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" t="s">
         <v>3</v>
+      </c>
+      <c r="E64" t="s">
+        <v>26</v>
       </c>
       <c r="H64" s="1">
         <v>44184</v>
@@ -1655,14 +2073,17 @@
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B65" s="2">
+      <c r="B65" s="1">
         <v>44128</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="D65" t="s">
         <v>16</v>
+      </c>
+      <c r="E65" t="s">
+        <v>26</v>
       </c>
       <c r="H65" s="1">
         <v>44185</v>
@@ -1673,14 +2094,17 @@
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B66" s="2">
+      <c r="B66" s="1">
         <v>44128</v>
       </c>
-      <c r="C66" s="3" t="s">
+      <c r="C66" t="s">
         <v>23</v>
       </c>
-      <c r="D66" s="3" t="s">
+      <c r="D66" t="s">
         <v>6</v>
+      </c>
+      <c r="E66" t="s">
+        <v>26</v>
       </c>
       <c r="H66" s="1">
         <v>44186</v>
@@ -1691,32 +2115,38 @@
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B67" s="2">
+      <c r="B67" s="1">
         <v>44129</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" t="s">
         <v>5</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" t="s">
         <v>21</v>
+      </c>
+      <c r="E67" t="s">
+        <v>26</v>
       </c>
       <c r="H67" s="1">
         <v>44191</v>
       </c>
       <c r="I67">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B68" s="2">
+      <c r="B68" s="1">
         <v>44136</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C68" t="s">
         <v>9</v>
       </c>
-      <c r="D68" s="3" t="s">
+      <c r="D68" t="s">
         <v>15</v>
+      </c>
+      <c r="E68" t="s">
+        <v>26</v>
       </c>
       <c r="H68" s="1">
         <v>44192</v>
@@ -1727,294 +2157,1541 @@
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B69" s="2">
+      <c r="B69" s="1">
         <v>44137</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="C69" t="s">
         <v>23</v>
       </c>
-      <c r="D69" s="3" t="s">
+      <c r="D69" t="s">
         <v>24</v>
       </c>
+      <c r="E69" t="s">
+        <v>26</v>
+      </c>
+      <c r="H69" s="1">
+        <v>44193</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B70" s="2">
+      <c r="B70" s="1">
         <v>44142</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C70" t="s">
         <v>6</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D70" t="s">
         <v>25</v>
       </c>
+      <c r="E70" t="s">
+        <v>26</v>
+      </c>
+      <c r="H70" s="1">
+        <v>43836</v>
+      </c>
+      <c r="I70">
+        <f t="shared" ref="I70:I74" si="1">COUNTIF(B$5:B$157,H70)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B71" s="2">
+      <c r="B71" s="1">
         <v>44142</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="C71" t="s">
         <v>7</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" t="s">
         <v>11</v>
       </c>
+      <c r="E71" t="s">
+        <v>26</v>
+      </c>
+      <c r="H71" s="1">
+        <v>43835</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B72" s="2">
+      <c r="B72" s="1">
         <v>44142</v>
       </c>
-      <c r="C72" s="3" t="s">
+      <c r="C72" t="s">
         <v>3</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D72" t="s">
         <v>23</v>
       </c>
+      <c r="E72" t="s">
+        <v>26</v>
+      </c>
+      <c r="H72" s="1">
+        <v>43834</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B73" s="2">
+      <c r="B73" s="1">
         <v>44143</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="C73" t="s">
         <v>5</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D73" t="s">
         <v>22</v>
       </c>
+      <c r="E73" t="s">
+        <v>26</v>
+      </c>
+      <c r="H73" s="1">
+        <v>43844</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B74" s="2">
+      <c r="B74" s="1">
         <v>44156</v>
       </c>
-      <c r="C74" s="3" t="s">
+      <c r="C74" t="s">
         <v>9</v>
       </c>
-      <c r="D74" s="3" t="s">
+      <c r="D74" t="s">
         <v>16</v>
       </c>
+      <c r="E74" t="s">
+        <v>26</v>
+      </c>
+      <c r="H74" s="1">
+        <v>43855</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B75" s="2">
+      <c r="B75" s="1">
         <v>44157</v>
       </c>
-      <c r="C75" s="3" t="s">
+      <c r="C75" t="s">
         <v>23</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="D75" t="s">
         <v>12</v>
       </c>
+      <c r="E75" t="s">
+        <v>26</v>
+      </c>
+      <c r="H75" s="1">
+        <v>43866</v>
+      </c>
+      <c r="I75">
+        <f>COUNTIF(B$5:B$157,H75)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B76" s="2">
+      <c r="B76" s="1">
         <v>44162</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C76" t="s">
         <v>6</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D76" t="s">
         <v>18</v>
       </c>
+      <c r="E76" t="s">
+        <v>26</v>
+      </c>
+      <c r="H76" s="1">
+        <v>43894</v>
+      </c>
+      <c r="I76">
+        <f t="shared" ref="I76:I95" si="2">COUNTIF(B$5:B$157,H76)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B77" s="2">
+      <c r="B77" s="1">
         <v>44164</v>
       </c>
-      <c r="C77" s="3" t="s">
+      <c r="C77" t="s">
         <v>7</v>
       </c>
-      <c r="D77" s="3" t="s">
+      <c r="D77" t="s">
         <v>9</v>
       </c>
+      <c r="E77" t="s">
+        <v>26</v>
+      </c>
+      <c r="H77" s="1">
+        <v>43893</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B78" s="2">
+      <c r="B78" s="1">
         <v>44164</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C78" t="s">
         <v>5</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="D78" t="s">
         <v>19</v>
       </c>
+      <c r="E78" t="s">
+        <v>26</v>
+      </c>
+      <c r="H78" s="1">
+        <v>44030</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B79" s="2">
+      <c r="B79" s="1">
         <v>44165</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" t="s">
         <v>3</v>
       </c>
-      <c r="D79" s="3" t="s">
+      <c r="D79" t="s">
         <v>22</v>
       </c>
+      <c r="E79" t="s">
+        <v>26</v>
+      </c>
+      <c r="H79" s="1">
+        <v>44044</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B80" s="2">
+      <c r="B80" s="1">
         <v>44170</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="C80" t="s">
         <v>3</v>
       </c>
-      <c r="D80" s="3" t="s">
+      <c r="D80" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B81" s="2">
+      <c r="E80" t="s">
+        <v>26</v>
+      </c>
+      <c r="H80" s="1">
+        <v>44089</v>
+      </c>
+      <c r="I80">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B81" s="1">
         <v>44170</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C81" t="s">
         <v>7</v>
       </c>
-      <c r="D81" s="3" t="s">
+      <c r="D81" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B82" s="2">
+      <c r="E81" t="s">
+        <v>26</v>
+      </c>
+      <c r="H81" s="1">
+        <v>44097</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B82" s="1">
         <v>44171</v>
       </c>
-      <c r="C82" s="3" t="s">
+      <c r="C82" t="s">
         <v>9</v>
       </c>
-      <c r="D82" s="3" t="s">
+      <c r="D82" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B83" s="2">
+      <c r="E82" t="s">
+        <v>26</v>
+      </c>
+      <c r="H82" s="1">
+        <v>44096</v>
+      </c>
+      <c r="I82">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B83" s="1">
         <v>44178</v>
       </c>
-      <c r="C83" s="3" t="s">
+      <c r="C83" t="s">
         <v>6</v>
       </c>
-      <c r="D83" s="3" t="s">
+      <c r="D83" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B84" s="2">
+      <c r="E83" t="s">
+        <v>26</v>
+      </c>
+      <c r="H83" s="1">
+        <v>44103</v>
+      </c>
+      <c r="I83">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B84" s="1">
         <v>44178</v>
       </c>
-      <c r="C84" s="3" t="s">
+      <c r="C84" t="s">
         <v>23</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="D84" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B85" s="2">
+      <c r="E84" t="s">
+        <v>26</v>
+      </c>
+      <c r="H84" s="1">
+        <v>44187</v>
+      </c>
+      <c r="I84">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B85" s="1">
         <v>44178</v>
       </c>
-      <c r="C85" s="3" t="s">
+      <c r="C85" t="s">
         <v>5</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D85" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B86" s="2">
+      <c r="E85" t="s">
+        <v>26</v>
+      </c>
+      <c r="H85" s="1">
+        <v>44131</v>
+      </c>
+      <c r="I85">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B86" s="1">
         <v>44181</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="C86" t="s">
         <v>5</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="D86" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B87" s="2">
+      <c r="E86" t="s">
+        <v>26</v>
+      </c>
+      <c r="H86" s="1">
+        <v>44138</v>
+      </c>
+      <c r="I86">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B87" s="1">
         <v>44181</v>
       </c>
-      <c r="C87" s="3" t="s">
+      <c r="C87" t="s">
         <v>23</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="D87" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B88" s="2">
+      <c r="E87" t="s">
+        <v>26</v>
+      </c>
+      <c r="H87" s="1">
+        <v>44167</v>
+      </c>
+      <c r="I87">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B88" s="1">
         <v>44181</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="C88" t="s">
         <v>3</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="D88" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B89" s="2">
+      <c r="E88" t="s">
+        <v>26</v>
+      </c>
+      <c r="H88" s="1">
+        <v>44177</v>
+      </c>
+      <c r="I88">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B89" s="1">
         <v>44184</v>
       </c>
-      <c r="C89" s="3" t="s">
+      <c r="C89" t="s">
         <v>6</v>
       </c>
-      <c r="D89" s="3" t="s">
+      <c r="D89" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B90" s="2">
+      <c r="E89" t="s">
+        <v>26</v>
+      </c>
+      <c r="H89" s="1">
+        <v>43847</v>
+      </c>
+      <c r="I89">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B90" s="1">
         <v>44185</v>
       </c>
-      <c r="C90" s="3" t="s">
+      <c r="C90" t="s">
         <v>9</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="D90" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B91" s="2">
+      <c r="E90" t="s">
+        <v>26</v>
+      </c>
+      <c r="H90" s="1">
+        <v>43876</v>
+      </c>
+      <c r="I90">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B91" s="1">
         <v>44186</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="C91" t="s">
         <v>7</v>
       </c>
-      <c r="D91" s="3" t="s">
+      <c r="D91" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B92" s="2">
+      <c r="E91" t="s">
+        <v>26</v>
+      </c>
+      <c r="H91" s="1">
+        <v>43887</v>
+      </c>
+      <c r="I91">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B92" s="1">
         <v>44191</v>
       </c>
-      <c r="C92" s="3" t="s">
+      <c r="C92" t="s">
         <v>23</v>
       </c>
-      <c r="D92" s="3" t="s">
+      <c r="D92" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B93" s="2">
+      <c r="E92" t="s">
+        <v>26</v>
+      </c>
+      <c r="H92" s="1">
+        <v>44009</v>
+      </c>
+      <c r="I92">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B93" s="1">
         <v>44191</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="C93" t="s">
         <v>5</v>
       </c>
-      <c r="D93" s="3" t="s">
+      <c r="D93" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B94" s="2">
+      <c r="E93" t="s">
+        <v>26</v>
+      </c>
+      <c r="H93" s="1">
+        <v>44015</v>
+      </c>
+      <c r="I93">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B94" s="1">
         <v>44192</v>
       </c>
-      <c r="C94" s="3" t="s">
+      <c r="C94" t="s">
         <v>3</v>
       </c>
-      <c r="D94" s="3" t="s">
+      <c r="D94" t="s">
         <v>15</v>
+      </c>
+      <c r="E94" t="s">
+        <v>26</v>
+      </c>
+      <c r="H94" s="1">
+        <v>44022</v>
+      </c>
+      <c r="I94">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B95" s="1">
+        <v>44193</v>
+      </c>
+      <c r="C95" t="s">
+        <v>6</v>
+      </c>
+      <c r="D95" t="s">
+        <v>21</v>
+      </c>
+      <c r="E95" t="s">
+        <v>26</v>
+      </c>
+      <c r="H95" s="1">
+        <v>44023</v>
+      </c>
+      <c r="I95">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B96" s="1">
+        <v>44193</v>
+      </c>
+      <c r="C96" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" t="s">
+        <v>22</v>
+      </c>
+      <c r="E96" t="s">
+        <v>26</v>
+      </c>
+      <c r="H96" s="1">
+        <v>43888</v>
+      </c>
+      <c r="I96">
+        <f>COUNTIF(B$5:B$157,H96)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B97" s="1">
+        <v>43836</v>
+      </c>
+      <c r="C97" t="s">
+        <v>5</v>
+      </c>
+      <c r="D97" t="s">
+        <v>25</v>
+      </c>
+      <c r="E97" t="s">
+        <v>30</v>
+      </c>
+      <c r="H97" s="1">
+        <v>44133</v>
+      </c>
+      <c r="I97">
+        <f t="shared" ref="I97:I109" si="3">COUNTIF(B$5:B$157,H97)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B98" s="1">
+        <v>43835</v>
+      </c>
+      <c r="C98" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" t="s">
+        <v>31</v>
+      </c>
+      <c r="E98" t="s">
+        <v>30</v>
+      </c>
+      <c r="H98" s="1">
+        <v>44140</v>
+      </c>
+      <c r="I98">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B99" s="1">
+        <v>43835</v>
+      </c>
+      <c r="C99" t="s">
+        <v>32</v>
+      </c>
+      <c r="D99" t="s">
+        <v>24</v>
+      </c>
+      <c r="E99" t="s">
+        <v>30</v>
+      </c>
+      <c r="H99" s="1">
+        <v>44168</v>
+      </c>
+      <c r="I99">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B100" s="1">
+        <v>43835</v>
+      </c>
+      <c r="C100" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" t="s">
+        <v>33</v>
+      </c>
+      <c r="E100" t="s">
+        <v>30</v>
+      </c>
+      <c r="H100" s="1">
+        <v>43880</v>
+      </c>
+      <c r="I100">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B101" s="1">
+        <v>43834</v>
+      </c>
+      <c r="C101" t="s">
+        <v>23</v>
+      </c>
+      <c r="D101" t="s">
+        <v>22</v>
+      </c>
+      <c r="E101" t="s">
+        <v>30</v>
+      </c>
+      <c r="H101" s="1">
+        <v>43886</v>
+      </c>
+      <c r="I101">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B102" s="1">
+        <v>43844</v>
+      </c>
+      <c r="C102" t="s">
+        <v>9</v>
+      </c>
+      <c r="D102" t="s">
+        <v>34</v>
+      </c>
+      <c r="E102" t="s">
+        <v>30</v>
+      </c>
+      <c r="H102" s="1">
+        <v>44124</v>
+      </c>
+      <c r="I102">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B103" s="1">
+        <v>43855</v>
+      </c>
+      <c r="C103" t="s">
+        <v>3</v>
+      </c>
+      <c r="D103" t="s">
+        <v>24</v>
+      </c>
+      <c r="E103" t="s">
+        <v>30</v>
+      </c>
+      <c r="H103" s="1">
+        <v>44139</v>
+      </c>
+      <c r="I103">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B104" s="1">
+        <v>43866</v>
+      </c>
+      <c r="C104" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104" t="s">
+        <v>13</v>
+      </c>
+      <c r="E104" t="s">
+        <v>30</v>
+      </c>
+      <c r="H104" s="1">
+        <v>44173</v>
+      </c>
+      <c r="I104">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B105" s="1">
+        <v>43894</v>
+      </c>
+      <c r="C105" t="s">
+        <v>9</v>
+      </c>
+      <c r="D105" t="s">
+        <v>14</v>
+      </c>
+      <c r="E105" t="s">
+        <v>30</v>
+      </c>
+      <c r="H105" s="1">
+        <v>44112</v>
+      </c>
+      <c r="I105">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B106" s="1">
+        <v>43893</v>
+      </c>
+      <c r="C106" t="s">
+        <v>7</v>
+      </c>
+      <c r="D106" t="s">
+        <v>10</v>
+      </c>
+      <c r="E106" t="s">
+        <v>30</v>
+      </c>
+      <c r="H106" s="1">
+        <v>44147</v>
+      </c>
+      <c r="I106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B107" s="1">
+        <v>44030</v>
+      </c>
+      <c r="C107" t="s">
+        <v>5</v>
+      </c>
+      <c r="D107" t="s">
+        <v>16</v>
+      </c>
+      <c r="E107" t="s">
+        <v>30</v>
+      </c>
+      <c r="H107" s="1">
+        <v>44115</v>
+      </c>
+      <c r="I107">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B108" s="1">
+        <v>44044</v>
+      </c>
+      <c r="C108" t="s">
+        <v>5</v>
+      </c>
+      <c r="D108" t="s">
+        <v>7</v>
+      </c>
+      <c r="E108" t="s">
+        <v>30</v>
+      </c>
+      <c r="H108" s="1">
+        <v>44118</v>
+      </c>
+      <c r="I108">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B109" s="1">
+        <v>44142</v>
+      </c>
+      <c r="C109" t="s">
+        <v>32</v>
+      </c>
+      <c r="D109" t="s">
+        <v>35</v>
+      </c>
+      <c r="E109" t="s">
+        <v>30</v>
+      </c>
+      <c r="H109" s="1">
+        <v>44153</v>
+      </c>
+      <c r="I109">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B110" s="1">
+        <v>44089</v>
+      </c>
+      <c r="C110" t="s">
+        <v>3</v>
+      </c>
+      <c r="D110" t="s">
+        <v>32</v>
+      </c>
+      <c r="E110" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B111" s="1">
+        <v>44097</v>
+      </c>
+      <c r="C111" t="s">
+        <v>7</v>
+      </c>
+      <c r="D111" t="s">
+        <v>37</v>
+      </c>
+      <c r="E111" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B112" s="1">
+        <v>44097</v>
+      </c>
+      <c r="C112" t="s">
+        <v>23</v>
+      </c>
+      <c r="D112" t="s">
+        <v>38</v>
+      </c>
+      <c r="E112" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B113" s="1">
+        <v>44096</v>
+      </c>
+      <c r="C113" t="s">
+        <v>3</v>
+      </c>
+      <c r="D113" t="s">
+        <v>39</v>
+      </c>
+      <c r="E113" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B114" s="1">
+        <v>44103</v>
+      </c>
+      <c r="C114" t="s">
+        <v>9</v>
+      </c>
+      <c r="D114" t="s">
+        <v>7</v>
+      </c>
+      <c r="E114" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B115" s="1">
+        <v>44187</v>
+      </c>
+      <c r="C115" t="s">
+        <v>5</v>
+      </c>
+      <c r="D115" t="s">
+        <v>16</v>
+      </c>
+      <c r="E115" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B116" s="1">
+        <v>44093</v>
+      </c>
+      <c r="C116" t="s">
+        <v>32</v>
+      </c>
+      <c r="D116" t="s">
+        <v>40</v>
+      </c>
+      <c r="E116" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B117" s="1">
+        <v>44107</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D117" t="s">
+        <v>42</v>
+      </c>
+      <c r="E117" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B118" s="1">
+        <v>44121</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D118" t="s">
+        <v>43</v>
+      </c>
+      <c r="E118" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B119" s="1">
+        <v>44131</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D119" t="s">
+        <v>44</v>
+      </c>
+      <c r="E119" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B120" s="1">
+        <v>44138</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D120" t="s">
+        <v>45</v>
+      </c>
+      <c r="E120" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B121" s="1">
+        <v>44167</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D121" t="s">
+        <v>46</v>
+      </c>
+      <c r="E121" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B122" s="1">
+        <v>44177</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D122" t="s">
+        <v>47</v>
+      </c>
+      <c r="E122" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B123" s="1">
+        <v>44191</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D123" t="s">
+        <v>35</v>
+      </c>
+      <c r="E123" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B124" s="1">
+        <v>43831</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D124" t="s">
+        <v>48</v>
+      </c>
+      <c r="E124" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B125" s="1">
+        <v>43841</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D125" t="s">
+        <v>24</v>
+      </c>
+      <c r="E125" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B126" s="1">
+        <v>43847</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D126" t="s">
+        <v>34</v>
+      </c>
+      <c r="E126" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B127" s="1">
+        <v>43852</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D127" t="s">
+        <v>23</v>
+      </c>
+      <c r="E127" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B128" s="1">
+        <v>43862</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D128" t="s">
+        <v>50</v>
+      </c>
+      <c r="E128" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B129" s="1">
+        <v>43862</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D129" t="s">
+        <v>51</v>
+      </c>
+      <c r="E129" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B130" s="1">
+        <v>43876</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D130" t="s">
+        <v>52</v>
+      </c>
+      <c r="E130" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B131" s="1">
+        <v>43876</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D131" t="s">
+        <v>50</v>
+      </c>
+      <c r="E131" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B132" s="1">
+        <v>43883</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D132" t="s">
+        <v>53</v>
+      </c>
+      <c r="E132" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B133" s="1">
+        <v>43887</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D133" t="s">
+        <v>54</v>
+      </c>
+      <c r="E133" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B134" s="1">
+        <v>43890</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D134" t="s">
+        <v>55</v>
+      </c>
+      <c r="E134" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B135" s="1">
+        <v>43897</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D135" t="s">
+        <v>34</v>
+      </c>
+      <c r="E135" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B136" s="1">
+        <v>44002</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D136" t="s">
+        <v>56</v>
+      </c>
+      <c r="E136" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B137" s="1">
+        <v>44009</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D137" t="s">
+        <v>57</v>
+      </c>
+      <c r="E137" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B138" s="1">
+        <v>44015</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D138" t="s">
+        <v>58</v>
+      </c>
+      <c r="E138" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B139" s="1">
+        <v>44016</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D139" t="s">
+        <v>59</v>
+      </c>
+      <c r="E139" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B140" s="1">
+        <v>44022</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D140" t="s">
+        <v>60</v>
+      </c>
+      <c r="E140" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B141" s="1">
+        <v>44023</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D141" t="s">
+        <v>61</v>
+      </c>
+      <c r="E141" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B142" s="1">
+        <v>44030</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D142" t="s">
+        <v>43</v>
+      </c>
+      <c r="E142" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B143" s="1">
+        <v>44030</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D143" t="s">
+        <v>38</v>
+      </c>
+      <c r="E143" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B144" s="1">
+        <v>43888</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D144" t="s">
+        <v>62</v>
+      </c>
+      <c r="E144" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B145" s="1">
+        <v>44133</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D145" t="s">
+        <v>64</v>
+      </c>
+      <c r="E145" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B146" s="1">
+        <v>44140</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D146" t="s">
+        <v>65</v>
+      </c>
+      <c r="E146" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B147" s="1">
+        <v>44168</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D147" t="s">
+        <v>66</v>
+      </c>
+      <c r="E147" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B148" s="1">
+        <v>43880</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D148" t="s">
+        <v>67</v>
+      </c>
+      <c r="E148" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B149" s="1">
+        <v>43886</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D149" t="s">
+        <v>69</v>
+      </c>
+      <c r="E149" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B150" s="1">
+        <v>44124</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D150" t="s">
+        <v>70</v>
+      </c>
+      <c r="E150" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B151" s="1">
+        <v>44139</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D151" t="s">
+        <v>71</v>
+      </c>
+      <c r="E151" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B152" s="1">
+        <v>44173</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D152" t="s">
+        <v>72</v>
+      </c>
+      <c r="E152" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B153" s="1">
+        <v>44112</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D153" t="s">
+        <v>74</v>
+      </c>
+      <c r="E153" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="154" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B154" s="1">
+        <v>44147</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D154" t="s">
+        <v>76</v>
+      </c>
+      <c r="E154" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="155" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B155" s="1">
+        <v>44115</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D155" t="s">
+        <v>77</v>
+      </c>
+      <c r="E155" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="156" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B156" s="1">
+        <v>44118</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D156" t="s">
+        <v>79</v>
+      </c>
+      <c r="E156" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="157" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B157" s="1">
+        <v>44153</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D157" t="s">
+        <v>80</v>
+      </c>
+      <c r="E157" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="H4:I68" xr:uid="{BBA24EEF-0B53-A64E-9F41-ED31D933E633}"/>
-  <conditionalFormatting sqref="I5:I68">
+  <conditionalFormatting sqref="I5:I109">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>